<commit_message>
Update service descriptions for checking and savings - consumer checking and savings - business checking and savings
</commit_message>
<xml_diff>
--- a/data/services.xlsx
+++ b/data/services.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jmlee\Documents\1. Academics\3. Spring\1. BigCo Studio\ct-studio-buildboard_bc\bigco\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC42E7C8-CECC-4378-9BE1-14ED1ACB56D2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B32487A8-5E08-4573-9E79-0E09FD42873E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="18470" windowHeight="11020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,14 +33,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>Consumer</t>
   </si>
   <si>
-    <t>Checking and savings</t>
-  </si>
-  <si>
     <t>Credit cards</t>
   </si>
   <si>
@@ -90,6 +87,12 @@
   </si>
   <si>
     <t>Financing</t>
+  </si>
+  <si>
+    <t>Consumer checking and savings</t>
+  </si>
+  <si>
+    <t>Business checking and savings</t>
   </si>
 </sst>
 </file>
@@ -419,7 +422,7 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -435,71 +438,71 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>5</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>18</v>
       </c>
       <c r="B2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C2" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="D2" t="s">
-        <v>1</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C3" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="D3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B4" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="D4" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="D6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>